<commit_message>
modified touch settings, added code to force LDO mode before hitting while(),
</commit_message>
<xml_diff>
--- a/doc/20190916-L10_QT8_Low_Power.xlsx
+++ b/doc/20190916-L10_QT8_Low_Power.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\microchip\mchp_fw\20190424-QT8\L10\saml10_qt8_lowpower\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFD5D7C-0B07-4D8C-A9A9-55485E1B8296}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99DA6D7-664E-4835-B0B7-C69924517C81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2850" yWindow="285" windowWidth="15105" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Targets" sheetId="2" r:id="rId1"/>
-    <sheet name="20190916" sheetId="1" r:id="rId2"/>
+    <sheet name="Sleep Power" sheetId="1" r:id="rId2"/>
+    <sheet name="Drift Rate" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>Current (uA)</t>
   </si>
@@ -59,6 +60,42 @@
   </si>
   <si>
     <t>High</t>
+  </si>
+  <si>
+    <t>16MHz</t>
+  </si>
+  <si>
+    <t>8MHz</t>
+  </si>
+  <si>
+    <t>4MHz</t>
+  </si>
+  <si>
+    <t>Sleep</t>
+  </si>
+  <si>
+    <t>PSU Mode</t>
+  </si>
+  <si>
+    <t>Buck</t>
+  </si>
+  <si>
+    <t>LDO</t>
+  </si>
+  <si>
+    <t>Single button Project Current</t>
+  </si>
+  <si>
+    <t>2D Touch Surface Project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drift calibration = 2 sec; comms dissabled; </t>
+  </si>
+  <si>
+    <t>Sleep power usage</t>
+  </si>
+  <si>
+    <t>PSU Mode in sleep</t>
   </si>
 </sst>
 </file>
@@ -216,7 +253,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'20190916'!$A$6:$A$13</c:f>
+              <c:f>'Sleep Power'!$A$9:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -249,7 +286,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'20190916'!$B$6:$B$13</c:f>
+              <c:f>'Sleep Power'!$B$9:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -695,7 +732,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'20190916'!$A$26:$A$31</c:f>
+              <c:f>'Drift Rate'!$A$6:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -722,7 +759,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'20190916'!$B$26:$B$31</c:f>
+              <c:f>'Drift Rate'!$B$6:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -750,7 +787,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E66A-42F0-AD85-AB9726BC2CD1}"/>
+              <c16:uniqueId val="{00000000-B7F3-491E-972C-754153503E74}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2247,13 +2284,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>6667</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>31432</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2279,25 +2316,30 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>20955</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96CEC315-7C5B-41D2-9504-342C096EE487}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DEF3503-4DF8-4DCB-9489-3A1069048641}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2311,7 +2353,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2586,7 +2628,7 @@
   <dimension ref="A2:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2661,10 +2703,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:E31"/>
+  <dimension ref="A3:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2676,10 +2718,314 @@
     <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
+      <c r="B7">
+        <v>3.3</v>
+      </c>
+      <c r="C7">
+        <v>3.3</v>
+      </c>
+      <c r="D7">
+        <v>1.8</v>
+      </c>
+      <c r="E7">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>86</v>
+      </c>
+      <c r="C9" s="1">
+        <f>$C$7*B9</f>
+        <v>283.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>54</v>
+      </c>
+      <c r="C10" s="1">
+        <f>$C$7*B10</f>
+        <v>178.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>32</v>
+      </c>
+      <c r="B11">
+        <v>32.5</v>
+      </c>
+      <c r="C11" s="1">
+        <f>$C$7*B11</f>
+        <v>107.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>64</v>
+      </c>
+      <c r="B12">
+        <v>23.7</v>
+      </c>
+      <c r="C12" s="1">
+        <f>$C$7*B12</f>
+        <v>78.209999999999994</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>128</v>
+      </c>
+      <c r="B13">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1">
+        <f>$C$7*B13</f>
+        <v>62.699999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>256</v>
+      </c>
+      <c r="B14">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1">
+        <f>$C$7*B14</f>
+        <v>56.099999999999994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>512</v>
+      </c>
+      <c r="B15">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1">
+        <f>$C$7*B15</f>
+        <v>52.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1024</v>
+      </c>
+      <c r="B16">
+        <v>15.3</v>
+      </c>
+      <c r="C16" s="1">
+        <f>$C$7*B16</f>
+        <v>50.49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46">
+        <v>3.3</v>
+      </c>
+      <c r="C46">
+        <v>3.3</v>
+      </c>
+      <c r="D46">
+        <v>1.8</v>
+      </c>
+      <c r="E46">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>0</v>
+      </c>
+      <c r="E47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48">
+        <v>29.86</v>
+      </c>
+      <c r="C48">
+        <f>B48*$C$46</f>
+        <v>98.537999999999997</v>
+      </c>
+      <c r="D48">
+        <v>31.02</v>
+      </c>
+      <c r="E48">
+        <f>D48*$E$46</f>
+        <v>55.835999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49">
+        <v>32.28</v>
+      </c>
+      <c r="C49">
+        <f>B49*$C$46</f>
+        <v>106.524</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <f>D49*$E$46</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>11</v>
+      </c>
+      <c r="B50">
+        <v>35.61</v>
+      </c>
+      <c r="C50">
+        <f>B50*$C$46</f>
+        <v>117.51299999999999</v>
+      </c>
+      <c r="D50">
+        <v>36.6</v>
+      </c>
+      <c r="E50">
+        <f>D50*$E$46</f>
+        <v>65.88000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51">
+        <v>17.7</v>
+      </c>
+      <c r="C51">
+        <f>B51*$C$46</f>
+        <v>58.41</v>
+      </c>
+      <c r="D51">
+        <v>10.37</v>
+      </c>
+      <c r="E51">
+        <f>D51*$E$46</f>
+        <v>18.666</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB481D1-832E-43F4-90C8-612B28E55598}">
+  <dimension ref="A4:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:N20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3.3</v>
       </c>
@@ -2695,7 +3041,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>0</v>
@@ -2712,200 +3058,73 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>8</v>
+        <v>1000</v>
       </c>
       <c r="B6">
-        <v>86</v>
-      </c>
-      <c r="C6" s="1">
+        <v>36</v>
+      </c>
+      <c r="C6">
         <f>$C$4*B6</f>
-        <v>283.8</v>
+        <v>118.8</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>16</v>
+        <v>2000</v>
       </c>
       <c r="B7">
-        <v>54</v>
-      </c>
-      <c r="C7" s="1">
-        <f t="shared" ref="C7:C13" si="0">$C$4*B7</f>
-        <v>178.2</v>
+        <v>32.700000000000003</v>
+      </c>
+      <c r="C7">
+        <f>$C$4*B7</f>
+        <v>107.91</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>32</v>
+        <v>4000</v>
       </c>
       <c r="B8">
-        <v>32.5</v>
-      </c>
-      <c r="C8" s="1">
-        <f t="shared" si="0"/>
-        <v>107.25</v>
+        <v>30.7</v>
+      </c>
+      <c r="C8">
+        <f>$C$4*B8</f>
+        <v>101.30999999999999</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>64</v>
+        <v>8000</v>
       </c>
       <c r="B9">
-        <v>23.7</v>
-      </c>
-      <c r="C9" s="1">
-        <f t="shared" si="0"/>
-        <v>78.209999999999994</v>
+        <v>29.7</v>
+      </c>
+      <c r="C9">
+        <f>$C$4*B9</f>
+        <v>98.009999999999991</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>128</v>
+        <v>16000</v>
       </c>
       <c r="B10">
-        <v>19</v>
-      </c>
-      <c r="C10" s="1">
-        <f t="shared" si="0"/>
-        <v>62.699999999999996</v>
+        <v>29.12</v>
+      </c>
+      <c r="C10">
+        <f>$C$4*B10</f>
+        <v>96.096000000000004</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>256</v>
+        <v>32000</v>
       </c>
       <c r="B11">
-        <v>17</v>
-      </c>
-      <c r="C11" s="1">
-        <f t="shared" si="0"/>
-        <v>56.099999999999994</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>512</v>
-      </c>
-      <c r="B12">
-        <v>16</v>
-      </c>
-      <c r="C12" s="1">
-        <f t="shared" si="0"/>
-        <v>52.8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1024</v>
-      </c>
-      <c r="B13">
-        <v>15.3</v>
-      </c>
-      <c r="C13" s="1">
-        <f t="shared" si="0"/>
-        <v>50.49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <v>3.3</v>
-      </c>
-      <c r="C24">
-        <v>3.3</v>
-      </c>
-      <c r="D24">
-        <v>1.8</v>
-      </c>
-      <c r="E24">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" t="s">
-        <v>0</v>
-      </c>
-      <c r="E25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>1000</v>
-      </c>
-      <c r="B26">
-        <v>36</v>
-      </c>
-      <c r="C26">
-        <f>$C$24*B26</f>
-        <v>118.8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>2000</v>
-      </c>
-      <c r="B27">
-        <v>32.700000000000003</v>
-      </c>
-      <c r="C27">
-        <f t="shared" ref="C27:C31" si="1">$C$24*B27</f>
-        <v>107.91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>4000</v>
-      </c>
-      <c r="B28">
-        <v>30.7</v>
-      </c>
-      <c r="C28">
-        <f t="shared" si="1"/>
-        <v>101.30999999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>8000</v>
-      </c>
-      <c r="B29">
-        <v>29.7</v>
-      </c>
-      <c r="C29">
-        <f t="shared" si="1"/>
-        <v>98.009999999999991</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>16000</v>
-      </c>
-      <c r="B30">
-        <v>29.12</v>
-      </c>
-      <c r="C30">
-        <f t="shared" si="1"/>
-        <v>96.096000000000004</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>32000</v>
-      </c>
-      <c r="B31">
         <v>28.91</v>
       </c>
-      <c r="C31">
-        <f t="shared" si="1"/>
+      <c r="C11">
+        <f>$C$4*B11</f>
         <v>95.402999999999992</v>
       </c>
     </row>

</xml_diff>

<commit_message>
stable, disabled driven shield to work with CCB, modified VREG settigns for 1.8V
</commit_message>
<xml_diff>
--- a/doc/20190916-L10_QT8_Low_Power.xlsx
+++ b/doc/20190916-L10_QT8_Low_Power.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\microchip\mchp_fw\20190424-QT8\L10\saml10_qt8_lowpower\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DB6F39-3846-4A49-963A-9A5954AD0600}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E641242-3D53-4468-9070-A5F938EF6D7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-12525" yWindow="-14640" windowWidth="15105" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14670" yWindow="-16320" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Targets" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>Current (uA)</t>
   </si>
@@ -62,50 +62,62 @@
     <t>High</t>
   </si>
   <si>
-    <t>16MHz</t>
-  </si>
-  <si>
-    <t>8MHz</t>
-  </si>
-  <si>
-    <t>4MHz</t>
-  </si>
-  <si>
-    <t>Sleep</t>
-  </si>
-  <si>
-    <t>PSU Mode</t>
-  </si>
-  <si>
-    <t>Buck</t>
-  </si>
-  <si>
-    <t>LDO</t>
-  </si>
-  <si>
-    <t>Single button Project Current</t>
-  </si>
-  <si>
     <t>2D Touch Surface Project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drift calibration = 2 sec; comms dissabled; </t>
   </si>
   <si>
     <t>Sleep power usage</t>
   </si>
   <si>
-    <t>PSU Mode in sleep</t>
+    <t xml:space="preserve">Drift calibration = 30 sec; comms dissabled; </t>
+  </si>
+  <si>
+    <t>RUNSTDBY | LPEFF | STDBYPL0</t>
+  </si>
+  <si>
+    <t>1, 1, 1</t>
+  </si>
+  <si>
+    <t>0, 0, 0</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Inst Current (uA)</t>
+  </si>
+  <si>
+    <t>Active Power</t>
+  </si>
+  <si>
+    <t>Inst Power (uW)</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Measured</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Scan Rate (ms)</t>
+  </si>
+  <si>
+    <t>Scan Freq (Hz)</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>? Does this use active or stdby, figure in active scan w/ stdby</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,16 +125,50 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -130,16 +176,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -168,92 +248,128 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>PTC</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> STDBY POWER vs SCANRATE</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1050" baseline="0"/>
+              <a:t>@ 1.8V</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1050"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="stacked"/>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sleep Power'!$I$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Current (uA)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
-            <a:ln w="22225" cap="rnd">
+            <a:ln w="34925" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent1">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
             </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>'Sleep Power'!$A$9:$A$16</c:f>
+              <c:f>'Sleep Power'!$A$10:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -286,33 +402,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sleep Power'!$B$9:$B$16</c:f>
+              <c:f>'Sleep Power'!$I$10:$I$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>86</c:v>
+                  <c:v>74.709999999999994</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>54</c:v>
+                  <c:v>38.380000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.5</c:v>
+                  <c:v>20.22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20.43</c:v>
+                  <c:v>11.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19</c:v>
+                  <c:v>6.39</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17</c:v>
+                  <c:v>5.3559999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16</c:v>
+                  <c:v>2.99</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15.3</c:v>
+                  <c:v>2.4790000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -324,10 +440,115 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sleep Power'!$J$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Power (uW)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sleep Power'!$A$10:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sleep Power'!$J$10:$J$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>134.47799999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>69.084000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36.396000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.98</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.501999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.6408000000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.3820000000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.4622000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AF92-487D-B68B-B1EC8FD290DB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
+          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="1"/>
+          <c:showVal val="0"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -344,92 +565,20 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>QTM_AUTOSCAN_TRIGGER_PERIOD (ms)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="10000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -441,7 +590,7 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -469,83 +618,19 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Current (uA)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -563,7 +648,7 @@
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -578,6 +663,43 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -598,20 +720,28 @@
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="dk1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -1181,6 +1311,502 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1729,569 +2355,20 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="15000"/>
-        <a:lumOff val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:miter lim="800000"/>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="22225" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-      <a:effectLst>
-        <a:glow rad="139700">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="14000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:effectRef>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr">
-          <a:lumMod val="60000"/>
-          <a:lumOff val="40000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:effectLst>
-        <a:glow rad="63500">
-          <a:schemeClr val="phClr">
-            <a:satMod val="175000"/>
-            <a:alpha val="25000"/>
-          </a:schemeClr>
-        </a:glow>
-      </a:effectLst>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="50000"/>
-          <a:lumOff val="50000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="65000"/>
-                <a:lumOff val="35000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="100000">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="75000"/>
-                <a:lumOff val="25000"/>
-                <a:alpha val="25000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="0">
-              <a:schemeClr val="dk1">
-                <a:lumMod val="65000"/>
-                <a:lumOff val="35000"/>
-                <a:alpha val="25000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="lt1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="85000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="25400" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1">
-          <a:lumMod val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="lt1">
-        <a:lumMod val="75000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>605790</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>24765</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>16192</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>300990</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>40957</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>329565</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2625,388 +2702,594 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF320401-232D-4B8D-A0C3-FDAC410CAE6C}">
-  <dimension ref="A2:C6"/>
+  <dimension ref="A2:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>1.8</v>
-      </c>
-      <c r="C2">
-        <v>1.8</v>
-      </c>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="11"/>
+      <c r="H2" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>0</v>
+      <c r="E3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="6">
+        <v>64</v>
+      </c>
+      <c r="C4" s="6">
+        <f>1/(B4/1000)</f>
+        <v>15.625</v>
+      </c>
+      <c r="D4" s="6">
         <v>72</v>
       </c>
-      <c r="C4">
-        <f>B4/$C$2</f>
+      <c r="E4" s="6">
+        <f>D4/1.8</f>
         <v>40</v>
       </c>
+      <c r="F4" s="7">
+        <f t="shared" ref="F4:F5" si="0">G4*1.8</f>
+        <v>19.98</v>
+      </c>
+      <c r="G4" s="7">
+        <v>11.1</v>
+      </c>
+      <c r="H4" s="8">
+        <f>(D4-F4)/D4</f>
+        <v>0.72249999999999992</v>
+      </c>
+      <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="6">
+        <v>32</v>
+      </c>
+      <c r="C5" s="6">
+        <f t="shared" ref="C5:C6" si="1">1/(B5/1000)</f>
+        <v>31.25</v>
+      </c>
+      <c r="D5" s="6">
         <v>540</v>
       </c>
-      <c r="C5">
-        <f t="shared" ref="C5:C6" si="0">B5/$C$2</f>
+      <c r="E5" s="6">
+        <f t="shared" ref="E5:E6" si="2">D5/1.8</f>
         <v>300</v>
       </c>
+      <c r="F5" s="7">
+        <f t="shared" si="0"/>
+        <v>36.396000000000001</v>
+      </c>
+      <c r="G5" s="7">
+        <v>20.22</v>
+      </c>
+      <c r="H5" s="8">
+        <f t="shared" ref="H5:I6" si="3">(D5-F5)/D5</f>
+        <v>0.93259999999999998</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="6">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="D6" s="6">
         <v>3600</v>
       </c>
-      <c r="C6">
-        <f t="shared" si="0"/>
+      <c r="E6" s="6">
+        <f t="shared" si="2"/>
         <v>2000</v>
       </c>
+      <c r="F6" s="7">
+        <f>G6*1.8</f>
+        <v>2048.4</v>
+      </c>
+      <c r="G6" s="7">
+        <v>1138</v>
+      </c>
+      <c r="H6" s="8">
+        <f t="shared" si="3"/>
+        <v>0.43099999999999999</v>
+      </c>
+      <c r="I6" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:E51"/>
+  <dimension ref="A3:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="D7">
         <v>3.3</v>
       </c>
-      <c r="C7">
+      <c r="F7">
         <v>3.3</v>
       </c>
-      <c r="D7">
+      <c r="H7">
         <v>1.8</v>
       </c>
-      <c r="E7">
+      <c r="J7">
         <v>1.8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9">
+        <v>380.7</v>
+      </c>
+      <c r="J9">
+        <f>I9*$J$7</f>
+        <v>685.26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>86</v>
-      </c>
-      <c r="C9" s="1">
-        <f t="shared" ref="C9:C16" si="0">$C$7*B9</f>
-        <v>283.8</v>
+      <c r="B10">
+        <f>1/(A10/1000)</f>
+        <v>125</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <f>C10*$D$7</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" ref="F10:F17" si="0">$F$7*E10</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1.1859999999999999</v>
+      </c>
+      <c r="H10" s="2">
+        <f>G10*$H$7</f>
+        <v>2.1347999999999998</v>
+      </c>
+      <c r="I10" s="2">
+        <v>74.709999999999994</v>
+      </c>
+      <c r="J10">
+        <f>I10*$J$7</f>
+        <v>134.47799999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>16</v>
       </c>
-      <c r="B10">
-        <v>54</v>
-      </c>
-      <c r="C10" s="1">
+      <c r="B11">
+        <f t="shared" ref="B11:B17" si="1">1/(A11/1000)</f>
+        <v>62.5</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" ref="D11:D17" si="2">C11*$D$7</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
         <f t="shared" si="0"/>
-        <v>178.2</v>
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1.1859999999999999</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" ref="H11:H17" si="3">G11*$H$7</f>
+        <v>2.1347999999999998</v>
+      </c>
+      <c r="I11" s="2">
+        <v>38.380000000000003</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ref="J11:J17" si="4">I11*$J$7</f>
+        <v>69.084000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>32</v>
       </c>
-      <c r="B11">
-        <v>32.5</v>
-      </c>
-      <c r="C11" s="1">
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>31.25</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
         <f t="shared" si="0"/>
-        <v>107.25</v>
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1.1859999999999999</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="3"/>
+        <v>2.1347999999999998</v>
+      </c>
+      <c r="I12" s="2">
+        <v>20.22</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="4"/>
+        <v>36.396000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>64</v>
       </c>
-      <c r="B12">
-        <v>20.43</v>
-      </c>
-      <c r="C12" s="1">
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>15.625</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
         <f t="shared" si="0"/>
-        <v>67.418999999999997</v>
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1.1859999999999999</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="3"/>
+        <v>2.1347999999999998</v>
+      </c>
+      <c r="I13" s="2">
+        <v>11.1</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="4"/>
+        <v>19.98</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>128</v>
       </c>
-      <c r="B13">
-        <v>19</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>7.8125</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0</v>
+      </c>
+      <c r="D14" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0</v>
+      </c>
+      <c r="F14" s="2">
         <f t="shared" si="0"/>
-        <v>62.699999999999996</v>
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1.1859999999999999</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="3"/>
+        <v>2.1347999999999998</v>
+      </c>
+      <c r="I14" s="2">
+        <v>6.39</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="4"/>
+        <v>11.501999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>256</v>
       </c>
-      <c r="B14">
-        <v>17</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>3.90625</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0</v>
+      </c>
+      <c r="F15" s="2">
         <f t="shared" si="0"/>
-        <v>56.099999999999994</v>
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1.1859999999999999</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="3"/>
+        <v>2.1347999999999998</v>
+      </c>
+      <c r="I15" s="2">
+        <v>5.3559999999999999</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="4"/>
+        <v>9.6408000000000005</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>512</v>
       </c>
-      <c r="B15">
-        <v>16</v>
-      </c>
-      <c r="C15" s="1">
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>1.953125</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0</v>
+      </c>
+      <c r="D16" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0</v>
+      </c>
+      <c r="F16" s="2">
         <f t="shared" si="0"/>
-        <v>52.8</v>
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1.1859999999999999</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="3"/>
+        <v>2.1347999999999998</v>
+      </c>
+      <c r="I16" s="2">
+        <v>2.99</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="4"/>
+        <v>5.3820000000000006</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>1024</v>
       </c>
-      <c r="B16">
-        <v>15.3</v>
-      </c>
-      <c r="C16" s="1">
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>0.9765625</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0</v>
+      </c>
+      <c r="F17" s="2">
         <f t="shared" si="0"/>
-        <v>50.49</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>13</v>
-      </c>
-      <c r="B45" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" t="s">
-        <v>14</v>
-      </c>
-      <c r="D45" t="s">
-        <v>15</v>
-      </c>
-      <c r="E45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>4</v>
-      </c>
-      <c r="B46">
-        <v>3.3</v>
-      </c>
-      <c r="C46">
-        <v>3.3</v>
-      </c>
-      <c r="D46">
-        <v>1.8</v>
-      </c>
-      <c r="E46">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>0</v>
-      </c>
-      <c r="C47" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" t="s">
-        <v>0</v>
-      </c>
-      <c r="E47" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>9</v>
-      </c>
-      <c r="B48">
-        <v>29.86</v>
-      </c>
-      <c r="C48">
-        <f>B48*$C$46</f>
-        <v>98.537999999999997</v>
-      </c>
-      <c r="D48">
-        <v>31.02</v>
-      </c>
-      <c r="E48">
-        <f>D48*$E$46</f>
-        <v>55.835999999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>10</v>
-      </c>
-      <c r="B49">
-        <v>32.28</v>
-      </c>
-      <c r="C49">
-        <f>B49*$C$46</f>
-        <v>106.524</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
-      </c>
-      <c r="E49">
-        <f>D49*$E$46</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>11</v>
-      </c>
-      <c r="B50">
-        <v>35.61</v>
-      </c>
-      <c r="C50">
-        <f>B50*$C$46</f>
-        <v>117.51299999999999</v>
-      </c>
-      <c r="D50">
-        <v>36.6</v>
-      </c>
-      <c r="E50">
-        <f>D50*$E$46</f>
-        <v>65.88000000000001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>12</v>
-      </c>
-      <c r="B51">
-        <v>17.7</v>
-      </c>
-      <c r="C51">
-        <f>B51*$C$46</f>
-        <v>58.41</v>
-      </c>
-      <c r="D51">
-        <v>10.37</v>
-      </c>
-      <c r="E51">
-        <f>D51*$E$46</f>
-        <v>18.666</v>
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>1.1859999999999999</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="3"/>
+        <v>2.1347999999999998</v>
+      </c>
+      <c r="I17" s="2">
+        <v>2.4790000000000001</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="4"/>
+        <v>4.4622000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>